<commit_message>
Updated on 12 May 2021
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Test_scenarios.xlsx
+++ b/src/main/resources/TestData/Test_scenarios.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="125">
   <si>
     <t xml:space="preserve">Scenario One - Dates </t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>

</xml_diff>